<commit_message>
fixed cut and paste typos
</commit_message>
<xml_diff>
--- a/scheme/ts-115-conformity-assessement-workbook.xlsx
+++ b/scheme/ts-115-conformity-assessement-workbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="1-3 Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,6 +52,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DGSI TS/115:2023 </t>
     </r>
@@ -60,6 +61,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">was prepared by the Digital Governance Standards Institute Technical Committee on digital credentials. The specification was approved by an expert committee and is intended to support a prototype conformity assessment program for digital credentials and digital trust services.</t>
     </r>
@@ -440,13 +442,13 @@
     <t xml:space="preserve">9.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">he Issuer Component shall identify the Issuer of the digital credential.</t>
+    <t xml:space="preserve">The Issuer Component shall identify the Issuer of the digital credential.</t>
   </si>
   <si>
     <t xml:space="preserve">9.1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">he Issuer Component shall be able to create a decentralized identifier for the Issuer, in 
+    <t xml:space="preserve">The Issuer Component shall be able to create a decentralized identifier for the Issuer, in 
 accordance with Section 8.</t>
   </si>
   <si>
@@ -465,7 +467,7 @@
     <t xml:space="preserve">9.1.4</t>
   </si>
   <si>
-    <t xml:space="preserve">he Issuer Component shall protect the digital credential, source data for the digital credential 
+    <t xml:space="preserve">The Issuer Component shall protect the digital credential, source data for the digital credential 
 and all other sensitive data, including personally identifiable information (PII) and personal 
 information (PI), in accordance with Section 6 of this Specification.</t>
   </si>
@@ -490,7 +492,7 @@
     <t xml:space="preserve">9.1.7</t>
   </si>
   <si>
-    <t xml:space="preserve">he Issuer Component shall be designed to create and update claims with respect to the 
+    <t xml:space="preserve">The Issuer Component shall be designed to create and update claims with respect to the 
 Subject(s) resulting from identity linking, identity verification, identity evidence determination, 
 and identity continuity processes of the Issuer in accordance with CAN/CIOSC 103-1.</t>
   </si>
@@ -889,14 +891,14 @@
     <t xml:space="preserve">11.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">he Verifier Component shall process digital credentials, in accordance with the general 
+    <t xml:space="preserve">The Verifier Component shall process digital credentials, in accordance with the general 
 characteristics specified in Subsection 5.1 of this Specification. </t>
   </si>
   <si>
     <t xml:space="preserve">11.1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">he Verifier Component shall ensure all digital credential data and all other sensitive data, 
+    <t xml:space="preserve">The Verifier Component shall ensure all digital credential data and all other sensitive data, 
 including personally identifiable information (PII) and personal information (PI), are protected 
 in accordance with Section 6 of this Specification.</t>
   </si>
@@ -904,14 +906,14 @@
     <t xml:space="preserve">11.1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">he Verifier Component shall conform to the Harmonized European Standard on Accessibility 
+    <t xml:space="preserve">The Verifier Component shall conform to the Harmonized European Standard on Accessibility 
 requirements for ICT products and services (EN 301-549).</t>
   </si>
   <si>
     <t xml:space="preserve">11.1.4</t>
   </si>
   <si>
-    <t xml:space="preserve">he Verifier Component shall provide support for official languages of the jurisdiction, and 
+    <t xml:space="preserve">The Verifier Component shall provide support for official languages of the jurisdiction, and 
 should provide support for additional languages (e.g., Indigenous languages).</t>
   </si>
   <si>
@@ -921,7 +923,7 @@
     <t xml:space="preserve">11.1.5</t>
   </si>
   <si>
-    <t xml:space="preserve">he Verifier Component shall have the capability to request from the Holder Component the 
+    <t xml:space="preserve">The Verifier Component shall have the capability to request from the Holder Component the 
 sharing of digital credential data, in whole, in part, or as a derivation. </t>
   </si>
   <si>
@@ -1041,6 +1043,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1062,18 +1065,21 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1216,11 +1222,11 @@
   </sheetPr>
   <dimension ref="B2:B24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73.5"/>
@@ -1330,12 +1336,12 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="89.06"/>
@@ -1615,13 +1621,13 @@
   </sheetPr>
   <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B140" activeCellId="0" sqref="B140"/>
+      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="78.64"/>
@@ -2752,7 +2758,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.83"/>
   </cols>

</xml_diff>